<commit_message>
Updated with Balloon insuflator link
</commit_message>
<xml_diff>
--- a/docs/BoM.xlsx
+++ b/docs/BoM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfreitas\Google Drive\CSW\Innovation&amp;Enterpreneurship\Balloon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfreitas\Google Drive\CSW\Innovation&amp;Enterpreneurship\Balloon\GitRepository\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -152,9 +152,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>Bocal Enchimento balão</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
   </si>
   <si>
     <t>http://pt.rs-online.com/web/p/modulos-de-video/9132664/?origin=PSF_437599|rel</t>
-  </si>
-  <si>
-    <t>3D Printed, source TBD (estimated around 45€)</t>
   </si>
   <si>
     <t>Item #</t>
@@ -236,6 +230,13 @@
   <si>
     <t>Items #23 and #24 can be bought together</t>
   </si>
+  <si>
+    <t>Model available in: http://www.thingiverse.com/thing:268080
+Can be 3D Printed, source of printing TBD (estimated around 45€ in 3DHubs)</t>
+  </si>
+  <si>
+    <t>Balloon insufflator (for HAB applications)</t>
+  </si>
 </sst>
 </file>
 
@@ -245,7 +246,7 @@
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -397,6 +398,90 @@
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -405,90 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -774,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -786,692 +787,692 @@
     <col min="4" max="4" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="14" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15" style="14" customWidth="1"/>
+    <col min="7" max="7" width="11" style="11" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="15" style="11" customWidth="1"/>
     <col min="10" max="10" width="38.42578125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>45</v>
+      <c r="J3" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="13">
         <v>34.08</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="13">
         <f>E4*G4</f>
         <v>68.16</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="13">
+      <c r="B5" s="31"/>
+      <c r="C5" s="10">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="13">
         <v>59.37</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="13">
         <f>E5*G5</f>
         <v>118.74</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="8"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="13">
+      <c r="B6" s="31"/>
+      <c r="C6" s="10">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="14">
         <v>54.94</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="13">
         <f>E6*G6</f>
         <v>109.88</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="8"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="13">
+      <c r="B7" s="31"/>
+      <c r="C7" s="10">
         <v>4</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="8"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="13">
+      <c r="B8" s="31"/>
+      <c r="C8" s="10">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="13">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:10" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="10">
         <v>6</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="17">
+      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="14">
         <v>45</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="13">
         <f>E9*G9</f>
         <v>45</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="8"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="10">
         <v>7</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="14">
         <v>33.1</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="13">
         <f>E10*G10</f>
         <v>33.1</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>52</v>
+      <c r="I10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="13">
+      <c r="B11" s="31"/>
+      <c r="C11" s="10">
         <v>8</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="17">
+      <c r="G11" s="14">
         <v>8.68</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <f>E11*G11</f>
         <v>8.68</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>52</v>
+      <c r="I11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="13">
+      <c r="B12" s="31"/>
+      <c r="C12" s="10">
         <v>9</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>17.989999999999998</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <f>E12*G12</f>
         <v>17.989999999999998</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="31"/>
+      <c r="C13" s="10">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="13">
-        <v>10</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="6"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="13">
+      <c r="B14" s="31"/>
+      <c r="C14" s="10">
         <v>11</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="17">
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="14">
         <v>23.09</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="13">
         <f>E14*G14</f>
         <v>23.09</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>52</v>
+      <c r="I14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="115.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="13">
+      <c r="B15" s="31"/>
+      <c r="C15" s="10">
         <v>12</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="9">
-        <v>1</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="14">
         <v>183.53</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="13">
         <f>E15*G15</f>
         <v>183.53</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="26" t="s">
-        <v>64</v>
+      <c r="I15" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="13">
+      <c r="B16" s="31"/>
+      <c r="C16" s="10">
         <v>13</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="9">
-        <v>1</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="22">
         <v>20.96</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="13">
         <f>E16*G16</f>
         <v>20.96</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="31"/>
+      <c r="C17" s="10">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="13">
-        <v>14</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="31"/>
+      <c r="C18" s="10">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="13">
-        <v>15</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="6">
-        <v>2</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18" s="6"/>
+      <c r="I18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="13">
+      <c r="B19" s="31"/>
+      <c r="C19" s="10">
         <v>16</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="17">
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="14">
         <v>125</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="13">
         <f>E19*G19</f>
         <v>125</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="13">
+      <c r="B20" s="32"/>
+      <c r="C20" s="10">
         <v>17</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-      <c r="F20" s="7" t="s">
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="7"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="2:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="10">
         <v>18</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-      <c r="F21" s="10" t="s">
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J21" s="6"/>
+      <c r="I21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="13">
+      <c r="B22" s="31"/>
+      <c r="C22" s="10">
         <v>19</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="10" t="s">
+      <c r="D22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="21">
         <v>40.71</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="13">
         <f>E22*G22</f>
         <v>40.71</v>
       </c>
-      <c r="I22" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="J22" s="6"/>
+      <c r="I22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="13">
+      <c r="B23" s="31"/>
+      <c r="C23" s="10">
         <v>20</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="9">
-        <v>1</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="23">
+      <c r="D23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="20">
         <v>12.48</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="20">
         <f>E23*G23</f>
         <v>12.48</v>
       </c>
-      <c r="I23" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23" s="18"/>
+      <c r="I23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="15"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="13">
+      <c r="B24" s="31"/>
+      <c r="C24" s="10">
         <v>21</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="13" t="s">
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" s="6"/>
+      <c r="I24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="13">
+      <c r="B25" s="31"/>
+      <c r="C25" s="10">
         <v>22</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="6">
-        <v>1</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="23">
+      <c r="D25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="20">
         <v>29.19</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="20">
         <f>E25*G25</f>
         <v>29.19</v>
       </c>
-      <c r="I25" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J25" s="6"/>
+      <c r="I25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="13">
+      <c r="B26" s="31"/>
+      <c r="C26" s="10">
         <v>23</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="6">
-        <v>1</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" s="23">
+      <c r="D26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="20">
         <v>57.44</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="20">
         <f>E26*G26</f>
         <v>57.44</v>
       </c>
-      <c r="I26" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>65</v>
+      <c r="I26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="13">
+      <c r="B27" s="32"/>
+      <c r="C27" s="10">
         <v>24</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="6">
-        <v>1</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="21">
+      <c r="G27" s="18">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H27" s="21">
+      <c r="H27" s="18">
         <f>E27*G27</f>
         <v>8.8000000000000007</v>
       </c>
-      <c r="I27" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>65</v>
+      <c r="I27" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="22">
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="19">
         <f>SUM(H4:H27)</f>
         <v>902.75</v>
       </c>
-      <c r="I28" s="28"/>
-      <c r="J28" s="29"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1496,8 +1497,9 @@
     <hyperlink ref="F26" r:id="rId14"/>
     <hyperlink ref="F27" r:id="rId15"/>
     <hyperlink ref="F19" r:id="rId16"/>
+    <hyperlink ref="F9" r:id="rId17" display="http://www.thingiverse.com/thing:268080"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated after reception of first batch of material
</commit_message>
<xml_diff>
--- a/docs/BoM.xlsx
+++ b/docs/BoM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfreitas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfreitas\Google Drive\Innovation&amp;Enterpreneurship\Balloon\GitRepository\repo\CSWspacepeek\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$3:$J$29</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>Item Description</t>
   </si>
@@ -146,9 +149,6 @@
     <t>Procurement priority</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>TNC Cable for Kenwood, Wouxun, Baofeng</t>
-  </si>
-  <si>
-    <t>TBC</t>
   </si>
   <si>
     <t>https://store.mobilinkd.com/products/kenwood-wouxun-baofeng-tnc-cable</t>
@@ -243,6 +240,15 @@
   <si>
     <t>http://www.generationrobots.com/en/401804-arduberry.html</t>
   </si>
+  <si>
+    <t>Deprecated</t>
+  </si>
+  <si>
+    <t>Not needed</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
 </sst>
 </file>
 
@@ -254,7 +260,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-816]_-;\-* #,##0.00\ [$€-816]_-;_-* &quot;-&quot;??\ [$€-816]_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +322,22 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,7 +429,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,9 +489,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -494,15 +513,6 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -523,6 +533,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -808,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -833,7 +879,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -854,39 +900,39 @@
         <v>39</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="41">
+        <v>1</v>
+      </c>
+      <c r="D4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3">
-        <v>2</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="39">
+        <v>0</v>
+      </c>
+      <c r="F4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="43">
         <v>34.08</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="43">
         <f>E4*G4</f>
-        <v>68.16</v>
+        <v>0</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="10">
         <v>2</v>
       </c>
@@ -907,12 +953,12 @@
         <v>118.74</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="10">
         <v>3</v>
       </c>
@@ -933,12 +979,12 @@
         <v>109.88</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="10">
         <v>4</v>
       </c>
@@ -949,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>10</v>
@@ -958,12 +1004,12 @@
         <v>10</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="10">
         <v>5</v>
       </c>
@@ -974,7 +1020,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>10</v>
@@ -983,23 +1029,23 @@
         <v>10</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="10">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="14">
         <v>45</v>
@@ -1009,12 +1055,12 @@
         <v>45</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="10">
@@ -1037,25 +1083,25 @@
         <v>33.1</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="10">
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="G11" s="14">
         <v>8.68</v>
@@ -1065,14 +1111,14 @@
         <v>8.68</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="10">
         <v>9</v>
       </c>
@@ -1093,12 +1139,12 @@
         <v>17.989999999999998</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="10">
         <v>10</v>
       </c>
@@ -1118,12 +1164,12 @@
         <v>20</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="10">
         <v>11</v>
       </c>
@@ -1134,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" s="14">
         <v>23.09</v>
@@ -1144,14 +1190,14 @@
         <v>23.09</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="115.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="10">
         <v>12</v>
       </c>
@@ -1172,14 +1218,14 @@
         <v>183.53</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="10">
         <v>13</v>
       </c>
@@ -1192,7 +1238,7 @@
       <c r="F16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="21">
         <v>20.96</v>
       </c>
       <c r="H16" s="13">
@@ -1200,14 +1246,14 @@
         <v>20.96</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="10">
         <v>14</v>
       </c>
@@ -1227,12 +1273,12 @@
         <v>20</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="10">
         <v>15</v>
       </c>
@@ -1252,38 +1298,38 @@
         <v>20</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
-      <c r="C19" s="10">
+      <c r="B19" s="37"/>
+      <c r="C19" s="41">
         <v>16</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="14">
+      <c r="E19" s="39">
+        <v>0</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="42">
         <v>125</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="43">
         <f>E19*G19</f>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="31"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="10">
         <v>17</v>
       </c>
@@ -1294,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>10</v>
@@ -1303,36 +1349,38 @@
         <v>10</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
-      <c r="C21" s="33">
+      <c r="B21" s="38"/>
+      <c r="C21" s="29">
         <v>25</v>
       </c>
-      <c r="D21" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="34">
-        <v>1</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="36">
+      <c r="D21" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="30">
+        <v>1</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="32">
         <v>48.06</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="33">
         <f>E21*G21</f>
         <v>48.06</v>
       </c>
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
+      <c r="I21" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="35"/>
     </row>
     <row r="22" spans="2:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="10">
@@ -1354,64 +1402,64 @@
         <v>20</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
-      <c r="C23" s="10">
+      <c r="B23" s="37"/>
+      <c r="C23" s="41">
         <v>19</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="39">
+        <v>0</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="44">
+        <v>40.71</v>
+      </c>
+      <c r="H23" s="43">
+        <f>E23*G23</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="37"/>
+      <c r="C24" s="41">
+        <v>20</v>
+      </c>
+      <c r="D24" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="21">
-        <v>40.71</v>
-      </c>
-      <c r="H23" s="13">
-        <f>E23*G23</f>
-        <v>40.71</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
-      <c r="C24" s="10">
-        <v>20</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="20">
+      <c r="E24" s="45">
+        <v>0</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="47">
         <v>12.48</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="47">
         <f>E24*G24</f>
-        <v>12.48</v>
+        <v>0</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="10">
         <v>21</v>
       </c>
@@ -1422,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>20</v>
@@ -1431,23 +1479,23 @@
         <v>20</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="10">
         <v>22</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="28" t="s">
-        <v>56</v>
+      <c r="F26" s="27" t="s">
+        <v>55</v>
       </c>
       <c r="G26" s="20">
         <v>29.19</v>
@@ -1457,23 +1505,23 @@
         <v>29.19</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="10">
         <v>23</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
       </c>
-      <c r="F27" s="28" t="s">
-        <v>58</v>
+      <c r="F27" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="G27" s="20">
         <v>57.44</v>
@@ -1483,25 +1531,25 @@
         <v>57.44</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="32"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="10">
         <v>24</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="28" t="s">
         <v>59</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>61</v>
       </c>
       <c r="G28" s="18">
         <v>8.8000000000000007</v>
@@ -1511,27 +1559,28 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="25"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="19">
         <f>SUM(H4:H28)</f>
-        <v>950.81000000000017</v>
-      </c>
-      <c r="I29" s="25"/>
-      <c r="J29" s="26"/>
+        <v>704.46</v>
+      </c>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25"/>
     </row>
   </sheetData>
+  <autoFilter ref="C3:J29"/>
   <mergeCells count="3">
     <mergeCell ref="B22:B28"/>
     <mergeCell ref="B4:B9"/>

</xml_diff>